<commit_message>
fix the bugs on tcpdfcustomize
</commit_message>
<xml_diff>
--- a/public/TCPDFCustomize/DATA/upload.xlsx
+++ b/public/TCPDFCustomize/DATA/upload.xlsx
@@ -1,28 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cosmos\Pictures\pdf\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE1842B-DC15-4C90-AC26-03A65128834E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="28275" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -75,44 +67,137 @@
     <t>fields_10</t>
   </si>
   <si>
+    <t>HASEGAWA</t>
+  </si>
+  <si>
+    <t>TAIZO</t>
+  </si>
+  <si>
+    <t>PARIS</t>
+  </si>
+  <si>
+    <t>MIKI PARIS OPTIQUE SARL</t>
+  </si>
+  <si>
+    <t>80 rue de rennes</t>
+  </si>
+  <si>
+    <t>MIKI</t>
+  </si>
+  <si>
+    <t>RENNES</t>
+  </si>
+  <si>
+    <t>RENAUD</t>
+  </si>
+  <si>
+    <t>Valerie</t>
+  </si>
+  <si>
+    <t>A.N.O.F.A.B.</t>
+  </si>
+  <si>
+    <t>TECHNOPOLE CITIS 1370, ROUTE D EPRON</t>
+  </si>
+  <si>
+    <t>AMORY</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>JARVILLE</t>
+  </si>
+  <si>
+    <t>SELARL DES DRS AMORY CATHERINE &amp; JEAN-LUC</t>
+  </si>
+  <si>
+    <t>70 AVENUE DE LA MALGRANGE</t>
+  </si>
+  <si>
+    <t>PEDINELLI</t>
+  </si>
+  <si>
+    <t>METZ</t>
+  </si>
+  <si>
+    <t>SELARL DE LA SEILLE</t>
+  </si>
+  <si>
+    <t>17 RUE DE LA CHARMINE</t>
+  </si>
+  <si>
+    <t>LEROUX</t>
+  </si>
+  <si>
+    <t>VINCENNES</t>
+  </si>
+  <si>
+    <t>CABINET LEROUX</t>
+  </si>
+  <si>
+    <t>32 RUE CELINE ROBERT</t>
+  </si>
+  <si>
+    <t>THOMAS</t>
+  </si>
+  <si>
+    <t>VERONIQUE</t>
+  </si>
+  <si>
+    <t>S.A.R.L. SECA</t>
+  </si>
+  <si>
+    <t>5 RUE PONSCARME</t>
+  </si>
+  <si>
+    <t>BAILLET</t>
+  </si>
+  <si>
+    <t>BORDEAUX</t>
+  </si>
+  <si>
+    <t>IMPRIMERIE BAILLET</t>
+  </si>
+  <si>
+    <t>249-251 RUE DU JARDIN PUBLIC BP 94</t>
+  </si>
+  <si>
+    <t>VALENTIN</t>
+  </si>
+  <si>
+    <t>Sofie</t>
+  </si>
+  <si>
+    <t>FRS FRANCE SARL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 AVENUE BERTIE ALBRECHT</t>
+  </si>
+  <si>
     <t>Steve</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>email01@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST 1 </t>
-  </si>
-  <si>
-    <t>TEST 6</t>
-  </si>
-  <si>
-    <t>TEST 7</t>
-  </si>
-  <si>
-    <t>TEST 8</t>
-  </si>
-  <si>
-    <t>TEST 9</t>
-  </si>
-  <si>
-    <t>TEST 10</t>
-  </si>
-  <si>
-    <t>"1/1/1985"</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>Adil</t>
+  </si>
+  <si>
+    <t>Nara</t>
+  </si>
+  <si>
+    <t>Damien</t>
+  </si>
+  <si>
+    <t>TEUGELS</t>
+  </si>
+  <si>
+    <t>HEROUVILLE ST CLAIR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,13 +226,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -155,19 +237,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -209,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -241,27 +315,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -293,24 +349,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -486,26 +524,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:L2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="9" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,62 +586,64 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4784515789</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1">
+        <v>75006</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>75006</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -622,17 +652,31 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>14209</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -641,31 +685,238 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>54140</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>57000</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>94300</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>75013</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>33327</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>33327</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>75008</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>